<commit_message>
Ajustes no código para gerar o arquivo em excel com os índices já calculados.
</commit_message>
<xml_diff>
--- a/Classificacao.xlsx
+++ b/Classificacao.xlsx
@@ -8,22 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49d5a67371d84b04/diversos antigos/Documentos/Projetos/projeto_b3_gitHub/empresas_b3_indices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94601FB-CB60-4798-A391-39D87711AFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F94601FB-CB60-4798-A391-39D87711AFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85237001-E649-4CFE-B43C-C933FBFD644B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{FD330A04-3708-4383-8E73-62810E85A537}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FD330A04-3708-4383-8E73-62810E85A537}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha2" sheetId="3" r:id="rId1"/>
-    <sheet name="Planilha1 (2)" sheetId="1" r:id="rId2"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId3"/>
+    <sheet name="classificacao" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Planilha1 (2)'!$A$1:$G$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">classificacao!$A$1:$G$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="308">
   <si>
     <t>SARAIVA LIVREIROS S.A. - EM RECUPERAÇÃO JUDICIAL</t>
   </si>
@@ -968,37 +963,14 @@
   </si>
   <si>
     <t>Restaurante e Similares</t>
-  </si>
-  <si>
-    <t>Rótulos de Linha</t>
-  </si>
-  <si>
-    <t>Total Geral</t>
-  </si>
-  <si>
-    <t>Contagem de CODIGOB3</t>
-  </si>
-  <si>
-    <t>Quantidade de Empresas</t>
-  </si>
-  <si>
-    <t>Subsetor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1014,7 +986,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1022,33 +994,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,949 +1015,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="gerson pereira de araujo" refreshedDate="45172.47925196759" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="91" xr:uid="{451C3ADC-D2A0-4A15-8508-158F710CCC62}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:G92" sheet="Planilha1 (2)"/>
-  </cacheSource>
-  <cacheFields count="7">
-    <cacheField name="SETOR_ECON" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="SUBSETOR" numFmtId="0">
-      <sharedItems count="8">
-        <s v="Construção Civil"/>
-        <s v="Tecidos, Vestuário e Calçados"/>
-        <s v="Utilidades Domésticas"/>
-        <s v="Automóveis e Motocicletas"/>
-        <s v="Hoteis e Restaurantes"/>
-        <s v="Viagens e Lazer"/>
-        <s v="Diversos"/>
-        <s v="Comércio"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="SEGMENTO" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="EMPRESA B3" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="CODIGOB3" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="ESTAGIO" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="NOME_CVM" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="91">
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="ALPHAVILLE"/>
-    <s v="AVLL"/>
-    <s v="NM             "/>
-    <s v="ALPHAVILLE S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="CONSTALIND"/>
-    <s v="CALI"/>
-    <m/>
-    <s v="CONSTRUTORA ADOLPHO LINDENBERG S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="CR2"/>
-    <s v="CRDE"/>
-    <s v="NM             "/>
-    <s v="FICA EMPREENDIMENTOS IMOBILIÁRIOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="CURYS/A"/>
-    <s v="CURY"/>
-    <s v="NM             "/>
-    <s v="CURY CONSTRUTORA E INCORPORADORA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="CYRELAREALT"/>
-    <s v="CYRE"/>
-    <s v="NM             "/>
-    <s v="CYRELA BRAZIL REALTY S.A.EMPREEND E PART"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="DIRECIONAL"/>
-    <s v="DIRR"/>
-    <s v="NM             "/>
-    <s v="DIRECIONAL ENGENHARIA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="EVEN"/>
-    <s v="EVEN"/>
-    <s v="NM             "/>
-    <s v="EVEN CONSTRUTORA E INCORPORADORA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="EZTEC"/>
-    <s v="EZTC"/>
-    <s v="NM             "/>
-    <s v="EZ TEC EMPREEND. E PARTICIPACOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="GAFISA"/>
-    <s v="GFSA"/>
-    <s v="NM             "/>
-    <s v="GAFISA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="HELBOR"/>
-    <s v="HBOR"/>
-    <s v="NM             "/>
-    <s v="HELBOR EMPREENDIMENTOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="INTERSA"/>
-    <s v="INNT"/>
-    <s v="MA"/>
-    <s v="INTER CONSTRUTORA E INCORPORADORA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="JHSFPART"/>
-    <s v="JHSF"/>
-    <s v="NM             "/>
-    <s v="JHSF PARTICIPACOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="JOAOFORTES"/>
-    <s v="JFEN"/>
-    <m/>
-    <s v="JOAO FORTES ENGENHARIA S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="KALLAS"/>
-    <s v="KLAS"/>
-    <m/>
-    <s v="KALLAS INCORPORAÇÕES E CONSTRUÇÕES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="LAVVI"/>
-    <s v="LAVV"/>
-    <s v="NM             "/>
-    <s v="LAVVI EMPREENDIMENTOS IMOBILIÁRIOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="MELNICK"/>
-    <s v="MELK"/>
-    <s v="NM             "/>
-    <s v="MELNICK DESENVOLVIMENTO IMOBILIÁRIO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="MITREREALTY"/>
-    <s v="MTRE"/>
-    <s v="NM             "/>
-    <s v="MITRE REALTY EMPREENDIMENTOS E PARTICIPAÇÕES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="MOURADUBEUX"/>
-    <s v="MDNE"/>
-    <s v="NM             "/>
-    <s v="MOURA DUBEUX ENGENHARIA S/A"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="MRV"/>
-    <s v="MRVE"/>
-    <s v="NM             "/>
-    <s v="MRV ENGENHARIA E PARTICIPACOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="PDGREALT"/>
-    <s v="PDGR"/>
-    <s v="NM             "/>
-    <s v="PDG REALTY S.A. EMPREEND E PARTICIPACOES"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="PLANOEPLANO"/>
-    <s v="PLPL"/>
-    <s v="NM             "/>
-    <s v="PLANO &amp; PLANO DESENVOLVIMENTO IMOBILIÁRIO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="RNI"/>
-    <s v="RDNI"/>
-    <s v="NM             "/>
-    <s v="RNI NEGÓCIOS IMOBILIÁRIOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="ROSSIRESID"/>
-    <s v="RSID"/>
-    <s v="NM             "/>
-    <s v="ROSSI RESIDENCIAL S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="TECNISA"/>
-    <s v="TCSA"/>
-    <s v="NM             "/>
-    <s v="TECNISA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="TEGRAINCORP"/>
-    <s v="TEGA"/>
-    <m/>
-    <s v="TEGRA INCORPORADORA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="TENDA"/>
-    <s v="TEND"/>
-    <s v="NM             "/>
-    <s v="CONSTRUTORA TENDA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="TRISUL"/>
-    <s v="TRIS"/>
-    <s v="NM             "/>
-    <s v="TRISUL S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="0"/>
-    <s v="Incorporações"/>
-    <s v="VIVER"/>
-    <s v="VIVR"/>
-    <s v="NM             "/>
-    <s v="VIVER INCORPORADORA E CONSTRUTORA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="CEDRO"/>
-    <s v="CEDO"/>
-    <s v="N1             "/>
-    <s v="CIA FIACAO TECIDOS CEDRO CACHOEIRA"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="COTEMINAS"/>
-    <s v="CTNM"/>
-    <m/>
-    <s v="CIA TECIDOS NORTE DE MINAS COTEMINAS"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="DOHLER"/>
-    <s v="DOHL"/>
-    <m/>
-    <s v="DOHLER S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="INDCATAGUAS"/>
-    <s v="CATA"/>
-    <m/>
-    <s v="CIA INDUSTRIAL CATAGUASES"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="KARSTEN"/>
-    <s v="CTKA"/>
-    <m/>
-    <s v="KARSTEN S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="PETTENATI"/>
-    <s v="PTNT"/>
-    <m/>
-    <s v="PETTENATI S.A. INDUSTRIA TEXTIL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="SANTANENSE"/>
-    <s v="CTSA"/>
-    <m/>
-    <s v="CIA TECIDOS SANTANENSE"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="SPRINGS"/>
-    <s v="SGPS"/>
-    <s v="NM             "/>
-    <s v="SPRINGS GLOBAL PARTICIPACOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="TEKA"/>
-    <s v="TEKA"/>
-    <m/>
-    <s v="TEKA-TECELAGEM KUEHNRICH S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Fios e Tecidos"/>
-    <s v="TEXRENAUX"/>
-    <s v="TXRX"/>
-    <m/>
-    <s v="TEXTIL RENAUXVIEW S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Vestuário"/>
-    <s v="TRACKFIELD"/>
-    <s v="TFCO"/>
-    <s v="N2"/>
-    <s v="TRACK &amp; FIELD CO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Calçados"/>
-    <s v="ALPARGATAS"/>
-    <s v="ALPA"/>
-    <s v="N1             "/>
-    <s v="ALPARGATAS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Calçados"/>
-    <s v="CAMBUCI"/>
-    <s v="CAMB"/>
-    <m/>
-    <s v="CAMBUCI S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Calçados"/>
-    <s v="GRENDENE"/>
-    <s v="GRND"/>
-    <s v="NM             "/>
-    <s v="GRENDENE S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Calçados"/>
-    <s v="VULCABRAS"/>
-    <s v="VULC"/>
-    <s v="NM             "/>
-    <s v="VULCABRAS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Acessórios"/>
-    <s v="MUNDIAL"/>
-    <s v="MNDL"/>
-    <m/>
-    <s v="MUNDIAL S.A. - PRODUTOS DE CONSUMO"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Acessórios"/>
-    <s v="TECHNOS"/>
-    <s v="TECN"/>
-    <s v="NM             "/>
-    <s v="TECHNOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="1"/>
-    <s v="Acessórios"/>
-    <s v="VIVARAS.A."/>
-    <s v="VIVA"/>
-    <s v="NM             "/>
-    <s v="VIVARA PARTICIPAÇÕES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="2"/>
-    <s v="Eletrodomésticos"/>
-    <s v="WHIRLPOOL"/>
-    <s v="WHRL"/>
-    <m/>
-    <s v="WHIRLPOOL S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="2"/>
-    <s v="Móveis"/>
-    <s v="UNICASA"/>
-    <s v="UCAS"/>
-    <s v="NM             "/>
-    <s v="UNICASA INDÚSTRIA DE MÓVEIS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="2"/>
-    <s v="Utensílios Domésticos"/>
-    <s v="HERCULES"/>
-    <s v="HETA"/>
-    <m/>
-    <s v="HERCULES S.A. FABRICA DE TALHERES"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="3"/>
-    <s v="Automóveis e Motocicletas"/>
-    <s v="IOCHP-MAXION"/>
-    <s v="MYPK"/>
-    <s v="NM             "/>
-    <s v="IOCHPE MAXION S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="3"/>
-    <s v="Automóveis e Motocicletas"/>
-    <s v="METALLEVE"/>
-    <s v="LEVE"/>
-    <s v="NM             "/>
-    <s v="MAHLE-METAL LEVE S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="3"/>
-    <s v="Automóveis e Motocicletas"/>
-    <s v="PLASCARPART"/>
-    <s v="PLAS"/>
-    <m/>
-    <s v="PLASCAR PARTICIPACOES INDUSTRIAIS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="4"/>
-    <s v="Hotelaria"/>
-    <s v="HOTEISOTHON"/>
-    <s v="HOOT"/>
-    <m/>
-    <s v="HOTEIS OTHON S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="4"/>
-    <s v="Restaurante e Similares"/>
-    <s v="IMCS/A"/>
-    <s v="MEAL"/>
-    <s v="NM             "/>
-    <s v="INTERNATIONAL MEAL COMPANY ALIMENTACAO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="4"/>
-    <s v="Restaurante e Similares"/>
-    <s v="ZAMPS.A."/>
-    <s v="ZAMP"/>
-    <s v="NM             "/>
-    <s v="ZAMP SA"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Bicicletas"/>
-    <s v="BICMONARK"/>
-    <s v="BMKS"/>
-    <m/>
-    <s v="BICICLETAS MONARK S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Brinquedos e Jogos"/>
-    <s v="ESTRELA"/>
-    <s v="ESTR"/>
-    <m/>
-    <s v="MANUFATURA DE BRINQUEDOS ESTRELA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Produção de Eventos e Shows"/>
-    <s v="SPTURIS"/>
-    <s v="AHEB"/>
-    <m/>
-    <s v="SAO PAULO TURISMO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Produção de Eventos e Shows"/>
-    <s v="TIMEFORFUN"/>
-    <s v="SHOW"/>
-    <s v="NM             "/>
-    <s v="T4F ENTRETENIMENTO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Viagens e Turismo"/>
-    <s v="CVCBRASIL"/>
-    <s v="CVCB"/>
-    <s v="NM             "/>
-    <s v="CVC BRASIL OPERADORA E AGÊNCIA DE VIAGENS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="5"/>
-    <s v="Atividades Esportivas"/>
-    <s v="SMARTFIT"/>
-    <s v="SMFT"/>
-    <s v="NM             "/>
-    <s v="SMARTFIT ESCOLA DE GINÁSTICA E DANÇA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="ANIMA"/>
-    <s v="ANIM"/>
-    <s v="NM             "/>
-    <s v="ANIMA HOLDING S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="BAHEMA"/>
-    <s v="BAHI"/>
-    <s v="MA"/>
-    <s v="BAHEMA EDUCAÇÃO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="COGNAON"/>
-    <s v="COGN"/>
-    <s v="NM             "/>
-    <s v="COGNA EDUCAÇÃO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="CRUZEIROEDU"/>
-    <s v="CSED"/>
-    <s v="NM             "/>
-    <s v="CRUZEIRO DO SUL EDUCACIONAL S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="SEREDUCA"/>
-    <s v="SEER"/>
-    <s v="NM             "/>
-    <s v="SER EDUCACIONAL S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Serviços Educacionais"/>
-    <s v="YDUQSPART"/>
-    <s v="YDUQ"/>
-    <s v="NM             "/>
-    <s v="YDUQS PARTICIPACOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Aluguel de carros"/>
-    <s v="LOCALIZA"/>
-    <s v="RENT"/>
-    <s v="NM             "/>
-    <s v="LOCALIZA RENT A CAR S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Aluguel de carros"/>
-    <s v="MAESTROLOC"/>
-    <s v="MSRO"/>
-    <s v="MA"/>
-    <s v="MAESTRO LOCADORA DE VEICULOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Aluguel de carros"/>
-    <s v="MOVIDA"/>
-    <s v="MOVI"/>
-    <s v="NM             "/>
-    <s v="MOVIDA LOCAÇÃO DE VEÍCULOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Aluguel de carros"/>
-    <s v="VAMOS"/>
-    <s v="VAMO"/>
-    <s v="NM             "/>
-    <s v="VAMOS LOCAÇÃO DE CAMINHÕES, MÁQUINAS E EQUIPAMENTOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="6"/>
-    <s v="Programas de Fidelização"/>
-    <s v="DOTZSA"/>
-    <s v="DOTZ"/>
-    <s v="NM             "/>
-    <s v="DOTZ S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="AREZZOCO"/>
-    <s v="ARZZ"/>
-    <s v="NM             "/>
-    <s v="AREZZO INDÚSTRIA E COMÉRCIO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="CEAMODAS"/>
-    <s v="CEAB"/>
-    <s v="NM             "/>
-    <s v="C&amp;A MODAS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="GRAZZIOTIN"/>
-    <s v="CGRA"/>
-    <m/>
-    <s v="GRAZZIOTIN S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="GRUPOSOMA"/>
-    <s v="SOMA"/>
-    <s v="NM             "/>
-    <s v="GRUPO DE MODA SOMA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="GUARARAPES"/>
-    <s v="GUAR"/>
-    <s v="NM             "/>
-    <s v="GUARARAPES CONFECCOES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="LOJASMARISA"/>
-    <s v="AMAR"/>
-    <s v="NM             "/>
-    <s v="MARISA LOJAS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="LOJASRENNER"/>
-    <s v="LREN"/>
-    <s v="NM             "/>
-    <s v="LOJAS RENNER S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Tecidos, Vestuário e Calçados"/>
-    <s v="VESTE"/>
-    <s v="VSTE"/>
-    <s v="NM             "/>
-    <s v="VESTE S.A. ESTILO"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Eletrodomésticos"/>
-    <s v="ALLIED"/>
-    <s v="ALLD"/>
-    <s v="NM             "/>
-    <s v="ALLIED TECNOLOGIA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Eletrodomésticos"/>
-    <s v="MAGAZLUIZA"/>
-    <s v="MGLU"/>
-    <s v="NM             "/>
-    <s v="MAGAZINE LUIZA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Eletrodomésticos"/>
-    <s v="VIA"/>
-    <s v="VIIA"/>
-    <s v="NM             "/>
-    <s v="VIA S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="AMERICANAS"/>
-    <s v="AMER"/>
-    <s v="NM             "/>
-    <s v="AMERICANAS S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="ESPACOLASER"/>
-    <s v="ESPA"/>
-    <s v="NM             "/>
-    <s v="MPM CORPÓREOS S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="GRUPOSBF"/>
-    <s v="SBFG"/>
-    <s v="NM             "/>
-    <s v="GRUPO SBF S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="LEBISCUIT"/>
-    <s v="LLBI"/>
-    <m/>
-    <s v="CVLB BRASIL S.A"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="PETZ"/>
-    <s v="PETZ"/>
-    <s v="NM             "/>
-    <s v="PET CENTER COMÉRCIO E PARTICIPAÇÕES S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="QUERO-QUERO"/>
-    <s v="LJQQ"/>
-    <s v="NM             "/>
-    <s v="LOJAS QUERO QUERO S.A."/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="SARAIVALIVR"/>
-    <s v="SLED"/>
-    <s v="N2             "/>
-    <s v="SARAIVA LIVREIROS S.A. - EM RECUPERAÇÃO JUDICIAL"/>
-  </r>
-  <r>
-    <s v="Consumo Cíclico"/>
-    <x v="7"/>
-    <s v="Produtos Diversos"/>
-    <s v="AMERICANAS"/>
-    <s v="AMER"/>
-    <s v="NM             "/>
-    <s v="LOJAS AMERICANAS S.A."/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C16619B9-8012-49D7-B7EB-1BF730DA6F01}" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="3"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Contagem de CODIGOB3" fld="4" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2305,174 +1313,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77BD6071-638D-4140-9958-F5B14BBAA249}">
-  <dimension ref="A3:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G6" s="3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G7" s="3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G8" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B9">
-        <v>18</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G10" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B12">
-        <v>91</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G12" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F13" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="G13" s="3">
-        <v>91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A9AA9E-E0A9-4DAD-BEF8-A028D456FBFA}">
   <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4537,16 +3382,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D7855B-1AA9-4E5D-BCF7-F6D61B61F12A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>